<commit_message>
changes in xlsx files
</commit_message>
<xml_diff>
--- a/drought/ibf_drought_impact_ea_v0.xlsx
+++ b/drought/ibf_drought_impact_ea_v0.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="impact_functions" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:v2="http://schemas.openxmlformats.org/spreadsheetml/2006/main/v2" mc:Ignorable="v2">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author> </author>
   </authors>
@@ -39,27 +39,6 @@
 Note on the damagefunctions tab: You can read only this tab with climada_damagefunctiuons_read and e.g. display all functions with climada_damagefunctions_plot. Replace existing damagefunctions in an encoded entity with these damagefunctions with climada_damagefunctions_map</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="false" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>16</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>2</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>3</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>13</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
     <comment ref="B1" authorId="0">
       <text>
@@ -74,27 +53,6 @@
           <t xml:space="preserve">The hazard intensity, i.e. has to correspond to the values in hazard.intensity</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="false" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>16</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>2</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>69</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>7</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
     <comment ref="C1" authorId="0">
       <text>
@@ -109,27 +67,6 @@
           <t xml:space="preserve">The Mean Damage Degree (the damage for a given intensity at an affected asset) - how strongly an asset is damaged. Range 0..1 (from none to total destruction)</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="false" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>16</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>2</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>56</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>6</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
     <comment ref="D1" authorId="0">
       <text>
@@ -144,27 +81,6 @@
           <t xml:space="preserve">The Percentage of Assets Affected  (the percentage of assets affected for a given hazard intensity) - how many assets are affected. Range 0..1 (from none affected to all affected)</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="false" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>16</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>2</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>61</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>1</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
     <comment ref="E1" authorId="0">
       <text>
@@ -179,27 +95,6 @@
           <t xml:space="preserve">the 2-digit peril identifier, e.g. TC for Tropical Cyclone wind, TS for surge, TR for rain, WS for European winter strom, EQ for earthquake. Matches with hazard.peril_ID. If empty, use the damage function irrespective of peril (i.e. the user needs to know which entity to expose to which peril)</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="false" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>52</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>2</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>-9</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>5</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
     <comment ref="F1" authorId="0">
       <text>
@@ -215,27 +110,6 @@
 The unit of the intensity, e.g. m/s for wind or MMI for earthquake. Please use SI units wherever possible.</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="false" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>2</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>69</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>8</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
     <comment ref="G1" authorId="0">
       <text>
@@ -251,27 +125,6 @@
 a free name, only used for annotation. Use only letters,  numbers and spaces, do not start with a letter.</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="false" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>37</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>2</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>58</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>2</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
@@ -317,11 +170,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -337,12 +191,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -412,7 +260,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,15 +270,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -458,7 +306,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.03"/>

</xml_diff>